<commit_message>
Added Add Client screen
</commit_message>
<xml_diff>
--- a/SoftwareAnalysisFinal/data.xlsx
+++ b/SoftwareAnalysisFinal/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mysait-my.sharepoint.com/personal/harry_jung_edu_sait_ca/Documents/Soft Analysis/SoftwareAnalysisFinal/SoftwareAnalysisFinal/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="52" documentId="11_F25DC773A252ABDACC104886495A69BA5BDE58E6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6374920B-7702-4EB3-B840-93A6EA638920}"/>
+  <xr:revisionPtr revIDLastSave="54" documentId="11_F25DC773A252ABDACC104886495A69BA5BDE58E6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6EEBF9F1-E1B2-4D12-9396-FCF1EBCE8331}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="CustomerInformation" sheetId="3" r:id="rId3"/>
     <sheet name="RentalInfo" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" fullCalcOnLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>category id</t>
   </si>
@@ -63,22 +63,10 @@
     <t>daily_rate</t>
   </si>
   <si>
-    <t>Hammer drill</t>
-  </si>
-  <si>
-    <t>Powerful drill for concrete and masonry</t>
-  </si>
-  <si>
-    <t>Chainsaw</t>
-  </si>
-  <si>
-    <t>Gas-powered chainsaw for cutting wood</t>
-  </si>
-  <si>
-    <t>Small Compressor</t>
-  </si>
-  <si>
-    <t>5 Gallon Compressor-Portable</t>
+    <t>501</t>
+  </si>
+  <si>
+    <t>50</t>
   </si>
   <si>
     <t>Brad Nailer</t>
@@ -87,6 +75,9 @@
     <t>Brad Nailer. Requires 3/4 to 1 1/2 Brad Nails</t>
   </si>
   <si>
+    <t>10.99</t>
+  </si>
+  <si>
     <t>customer_id</t>
   </si>
   <si>
@@ -151,19 +142,14 @@
   </si>
   <si>
     <t>cost</t>
-  </si>
-  <si>
-    <t>Lawn mower</t>
-  </si>
-  <si>
-    <t>Self-propelled lawn mower with mulching function</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -205,9 +191,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="1" applyFont="1" fillId="0" applyFill="0" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -218,13 +204,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" applyFont="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" applyFont="1" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" applyNumberFormat="1" fontId="2" applyFont="1" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" applyFont="1" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -519,7 +502,7 @@
     <col min="1" max="2" width="10.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -527,7 +510,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2">
       <c r="A2" s="2">
         <v>10</v>
       </c>
@@ -535,7 +518,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="3" ht="28.5">
       <c r="A3" s="2">
         <v>20</v>
       </c>
@@ -543,7 +526,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="4" ht="28.5">
       <c r="A4" s="2">
         <v>30</v>
       </c>
@@ -551,7 +534,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5">
       <c r="A5" s="2">
         <v>40</v>
       </c>
@@ -559,7 +542,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6">
       <c r="A6" s="2">
         <v>50</v>
       </c>
@@ -569,123 +552,57 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C155990-222F-450F-8567-C4ACB1FD99A5}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E6"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A1" t="s">
+    <row r="1">
+      <c r="A1" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="0" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A2" s="8">
-        <v>101</v>
-      </c>
-      <c r="B2" s="8">
-        <v>10</v>
-      </c>
-      <c r="C2" t="s">
+    <row r="2">
+      <c r="A2" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
+      <c r="B2" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="E2">
-        <v>25.99</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A3" s="8">
-        <v>201</v>
-      </c>
-      <c r="B3" s="8">
-        <v>20</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="C2" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D2" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="E3">
-        <v>49.99</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A4" s="8">
-        <v>202</v>
-      </c>
-      <c r="B4" s="8">
-        <v>20</v>
-      </c>
-      <c r="C4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E4">
-        <v>19.989999999999998</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A5" s="8">
-        <v>301</v>
-      </c>
-      <c r="B5" s="8">
-        <v>30</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="E2" s="0" t="s">
         <v>15</v>
-      </c>
-      <c r="D5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5">
-        <v>14.99</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A6" s="8">
-        <v>501</v>
-      </c>
-      <c r="B6" s="8">
-        <v>50</v>
-      </c>
-      <c r="C6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6">
-        <v>10.99</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
@@ -699,88 +616,89 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="10.46484375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.86328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.19921875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.06640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.19921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="1" width="10.46484375" customWidth="1"/>
+    <col min="2" max="2" bestFit="1" width="8.86328125" customWidth="1"/>
+    <col min="3" max="3" bestFit="1" width="9.19921875" customWidth="1"/>
+    <col min="4" max="4" bestFit="1" width="13.06640625" customWidth="1"/>
+    <col min="5" max="5" bestFit="1" width="13.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A1" t="s">
+    <row r="1">
+      <c r="A1" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="2">
+      <c r="A2" s="0">
+        <v>1001</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="D1" t="s">
+      <c r="C2" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="E1" t="s">
+      <c r="D2" s="0" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A2">
-        <v>1001</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="E2" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C2" t="s">
+    </row>
+    <row r="3">
+      <c r="A3" s="0">
+        <v>1002</v>
+      </c>
+      <c r="B3" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C3" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="D3" s="0" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A3">
-        <v>1002</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="E3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C3" t="s">
+    </row>
+    <row r="4">
+      <c r="A4" s="0">
+        <v>1003</v>
+      </c>
+      <c r="B4" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="D3" t="s">
+      <c r="C4" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="D4" s="0" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A4">
-        <v>1003</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="E4" s="4" t="s">
         <v>32</v>
-      </c>
-      <c r="C4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>35</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
-    <hyperlink ref="E3" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
-    <hyperlink ref="E4" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="E3" r:id="rId2"/>
+    <hyperlink ref="E4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
@@ -794,38 +712,38 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="7.59765625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.9296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.3984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.46484375" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="9.9296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.73046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="1" width="7.59765625" customWidth="1"/>
+    <col min="2" max="2" bestFit="1" width="9.9296875" customWidth="1"/>
+    <col min="3" max="3" bestFit="1" width="10.3984375" customWidth="1"/>
+    <col min="4" max="4" bestFit="1" width="11.46484375" customWidth="1"/>
+    <col min="5" max="6" bestFit="1" width="9.9296875" customWidth="1"/>
+    <col min="7" max="7" bestFit="1" width="6.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.4" x14ac:dyDescent="0.45">
+    <row r="1" ht="15.4">
       <c r="A1" s="5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="15.4" x14ac:dyDescent="0.45">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" ht="15.4">
       <c r="A2" s="5">
         <v>1000</v>
       </c>
@@ -848,7 +766,7 @@
         <v>149.97</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.4" x14ac:dyDescent="0.45">
+    <row r="3" ht="15.4">
       <c r="A3" s="5">
         <v>1001</v>
       </c>
@@ -873,5 +791,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>